<commit_message>
move existing files to cartesian sub folder
</commit_message>
<xml_diff>
--- a/mesh-interpolation/拟合点(1).xlsx
+++ b/mesh-interpolation/拟合点(1).xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\24538\Desktop\邻面成型片\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Dentist-Feng\mesh-interpolation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC6633B-B559-42E7-90C7-E3D62AFDC327}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8763E0-7865-4112-8D22-9E66847D25BE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30465" yWindow="1245" windowWidth="20910" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -606,18 +607,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -641,8 +642,12 @@
       <c r="D2">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>SQRT(B2 * B2 + C2 * C2)</f>
+        <v>4.5435999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -655,8 +660,12 @@
       <c r="D3">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" ref="E3:E61" si="0">SQRT(B3 * B3 + C3 * C3)</f>
+        <v>4.7126999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -669,8 +678,12 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4.7667999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -683,8 +696,12 @@
       <c r="D5">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>4.6435000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -697,8 +714,12 @@
       <c r="D6">
         <v>-1.96</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4.4265999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -711,8 +732,12 @@
       <c r="D7">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4.4408254424149574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -725,8 +750,12 @@
       <c r="D8">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>4.6075204839479555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -739,8 +768,12 @@
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>4.6223167351448344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -753,8 +786,12 @@
       <c r="D10">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>4.4861870591851165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -765,11 +802,14 @@
         <v>-4.0301</v>
       </c>
       <c r="D11">
-        <f>B14-1.96</f>
-        <v>0.22710000000000008</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-1.96</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>4.1722763594948988</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -782,8 +822,12 @@
       <c r="D12">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4.5288882366426311</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -796,8 +840,12 @@
       <c r="D13">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>4.5212724691175161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -810,8 +858,12 @@
       <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4.3741408322092239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -824,8 +876,12 @@
       <c r="D15">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>4.0961019152359963</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -838,8 +894,12 @@
       <c r="D16">
         <v>-1.96</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>3.6108980406541527</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -852,8 +912,12 @@
       <c r="D17">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>4.5700311268086571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -866,8 +930,12 @@
       <c r="D18">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>4.4698340964738277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -880,8 +948,12 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>4.1508582269212715</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -894,8 +966,12 @@
       <c r="D20">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>3.5404836534010431</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -906,11 +982,14 @@
         <v>-2.0886</v>
       </c>
       <c r="D21">
-        <f>B24-1.96</f>
-        <v>1.3117999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-1.96</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>2.9537971578969331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -923,8 +1002,12 @@
       <c r="D22">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>4.1027748622121596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -937,8 +1020,12 @@
       <c r="D23">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>4.0857076865581066</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -951,8 +1038,12 @@
       <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>3.7779619161659106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -965,8 +1056,12 @@
       <c r="D25">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>3.0256463656547834</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -979,8 +1074,12 @@
       <c r="D26">
         <v>-1.96</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>2.5604247303914249</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -993,8 +1092,12 @@
       <c r="D27">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>3.5627941801344627</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1007,8 +1110,12 @@
       <c r="D28">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>3.6626128433128171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1021,8 +1128,12 @@
       <c r="D29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>3.5028553795439517</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1035,8 +1146,12 @@
       <c r="D30">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>2.8405910441314846</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1047,11 +1162,14 @@
         <v>-0.60450000000000004</v>
       </c>
       <c r="D31">
-        <f>B34-1.96</f>
-        <v>1.339</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-1.96</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>2.3355847768813698</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1064,8 +1182,12 @@
       <c r="D32">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>3.2101000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1078,8 +1200,12 @@
       <c r="D33">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>3.4695999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1092,8 +1218,12 @@
       <c r="D34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>3.2989999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1106,8 +1236,12 @@
       <c r="D35">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>2.8569</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1120,8 +1254,12 @@
       <c r="D36">
         <v>-1.96</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>2.3369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1134,8 +1272,12 @@
       <c r="D37">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>3.1981625865487202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1148,8 +1290,12 @@
       <c r="D38">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>3.4634136512983837</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1162,8 +1308,12 @@
       <c r="D39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>3.3292486434629662</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1176,8 +1326,12 @@
       <c r="D40">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>2.9966123556442867</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1188,11 +1342,14 @@
         <v>0.64859999999999995</v>
       </c>
       <c r="D41">
-        <f>B44-1.96</f>
-        <v>1.1109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-1.96</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>2.5059900877697019</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1205,8 +1362,12 @@
       <c r="D42">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>3.4993765901943163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1219,8 +1380,12 @@
       <c r="D43">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>3.7064549437434149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1233,8 +1398,12 @@
       <c r="D44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>3.545927413244665</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1247,8 +1416,12 @@
       <c r="D45">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>3.2068257514246077</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1261,8 +1434,12 @@
       <c r="D46">
         <v>-1.96</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>2.7583114853112582</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1275,8 +1452,12 @@
       <c r="D47">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>3.8701368347902121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1289,8 +1470,12 @@
       <c r="D48">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>4.01763931183475</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1303,8 +1488,12 @@
       <c r="D49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>3.8969361824387114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1317,8 +1506,12 @@
       <c r="D50">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>3.5778896028245475</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1329,11 +1522,14 @@
         <v>2.3136000000000001</v>
       </c>
       <c r="D51">
-        <f>B54-1.96</f>
-        <v>0.20630000000000015</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-1.96</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>3.2719952093485714</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1346,8 +1542,12 @@
       <c r="D52">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>4.2626693807988438</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1360,8 +1560,12 @@
       <c r="D53">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>4.3886161509067989</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1374,8 +1578,12 @@
       <c r="D54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>4.3325639175896757</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1388,8 +1596,12 @@
       <c r="D55">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>4.0948492878248883</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1402,8 +1614,12 @@
       <c r="D56">
         <v>-1.96</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>3.7376010287348755</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1416,8 +1632,12 @@
       <c r="D57">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>4.4091457959564</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1430,8 +1650,12 @@
       <c r="D58">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>4.6658102758256259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -1444,8 +1668,12 @@
       <c r="D59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>4.6000740624472556</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -1458,8 +1686,12 @@
       <c r="D60">
         <v>-0.98</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>4.4519114243210183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -1472,6 +1704,10 @@
       <c r="D61">
         <f>B64-1.96</f>
         <v>-1.96</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>4.1321067193382115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>